<commit_message>
add fun to extract titles from links
</commit_message>
<xml_diff>
--- a/domains.xlsx
+++ b/domains.xlsx
@@ -2,34 +2,88 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+  <si>
+    <t>Search Word</t>
+  </si>
+  <si>
+    <t>Link Text</t>
+  </si>
+  <si>
+    <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغة</t>
+  </si>
+  <si>
+    <t>https://sabq.org/saudia/vhlt14pdwv</t>
+  </si>
+  <si>
+    <t>https://www.okaz.com.sa/news/local/2166479</t>
+  </si>
+  <si>
+    <t>https://www.tech-mag.net/260-%D9%85%D8%AA%D8%AE%D8%B5%D8%B5%D9%8B%D8%A7-%D8%B9%D8%A7%D9%84%D9%85%D9%8A%D9%8B%D8%A7-%D9%8A%D8%AA%D8%B1%D8%AC%D9%85%D9%88%D9%86-%D8%A3%D8%B3%D8%A6%D9%84%D8%A9-%D8%A3%D9%88%D9%84%D9%85%D8%A8%D9%8A/</t>
+  </si>
+  <si>
+    <t>https://al-hadath.com/post/75279</t>
+  </si>
+  <si>
+    <t>https://www.tilmass.info/?tag=%D9%84%D8%AD%D8%B1%D8%A7%D8%B7%D9%8A%D9%86</t>
+  </si>
+  <si>
+    <t>https://aldira.net/?p=26334</t>
+  </si>
+  <si>
+    <t>https://shababeks.com/2024/07/23/mr-129/</t>
+  </si>
+  <si>
+    <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغةsabq.org › محليات</t>
+  </si>
+  <si>
+    <t>260 متخصصاً عالمياً يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغةlocal ‹ news ‹ www.okaz.com.sa</t>
+  </si>
+  <si>
+    <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغةأخبار وتقارير ‹ www.tech-mag.net</t>
+  </si>
+  <si>
+    <t>قلل الاستهلاك وحسن الأداء.. نصيحتان من "المواصفات" عن "الاستخدام ...post ‹ al-hadath.com</t>
+  </si>
+  <si>
+    <t>لحراطين - موقع تلماس الإخباري... ‹ www.tilmass.info</t>
+  </si>
+  <si>
+    <t>"تعليم عسير" تحصل على 3 جوائز في الأولمبياد الوطني للإبداع بمجال ...... ‹ aldira.net</t>
+  </si>
+  <si>
+    <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغة ...</t>
+  </si>
   <si>
     <t>search link</t>
-  </si>
-  <si>
-    <t>https://www.spa.gov.sa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -42,7 +96,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -61,21 +114,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -371,58 +445,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A3:A9"/>
+      <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="1" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create a model to share data to wordpress site
</commit_message>
<xml_diff>
--- a/domains.xlsx
+++ b/domains.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Search Word</t>
   </si>
@@ -28,43 +28,7 @@
     <t>https://sabq.org/saudia/vhlt14pdwv</t>
   </si>
   <si>
-    <t>https://www.okaz.com.sa/news/local/2166479</t>
-  </si>
-  <si>
-    <t>https://www.tech-mag.net/260-%D9%85%D8%AA%D8%AE%D8%B5%D8%B5%D9%8B%D8%A7-%D8%B9%D8%A7%D9%84%D9%85%D9%8A%D9%8B%D8%A7-%D9%8A%D8%AA%D8%B1%D8%AC%D9%85%D9%88%D9%86-%D8%A3%D8%B3%D8%A6%D9%84%D8%A9-%D8%A3%D9%88%D9%84%D9%85%D8%A8%D9%8A/</t>
-  </si>
-  <si>
-    <t>https://al-hadath.com/post/75279</t>
-  </si>
-  <si>
-    <t>https://www.tilmass.info/?tag=%D9%84%D8%AD%D8%B1%D8%A7%D8%B7%D9%8A%D9%86</t>
-  </si>
-  <si>
-    <t>https://aldira.net/?p=26334</t>
-  </si>
-  <si>
-    <t>https://shababeks.com/2024/07/23/mr-129/</t>
-  </si>
-  <si>
     <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغةsabq.org › محليات</t>
-  </si>
-  <si>
-    <t>260 متخصصاً عالمياً يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغةlocal ‹ news ‹ www.okaz.com.sa</t>
-  </si>
-  <si>
-    <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغةأخبار وتقارير ‹ www.tech-mag.net</t>
-  </si>
-  <si>
-    <t>قلل الاستهلاك وحسن الأداء.. نصيحتان من "المواصفات" عن "الاستخدام ...post ‹ al-hadath.com</t>
-  </si>
-  <si>
-    <t>لحراطين - موقع تلماس الإخباري... ‹ www.tilmass.info</t>
-  </si>
-  <si>
-    <t>"تعليم عسير" تحصل على 3 جوائز في الأولمبياد الوطني للإبداع بمجال ...... ‹ aldira.net</t>
-  </si>
-  <si>
-    <t>260 متخصصًا عالميًا يترجمون أسئلة أولمبياد الكيمياء الدولي إلى 50 لغة ...</t>
   </si>
   <si>
     <t>search link</t>
@@ -448,7 +412,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +425,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -475,96 +439,32 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -578,14 +478,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>